<commit_message>
add some new functions
</commit_message>
<xml_diff>
--- a/BE/hix_lix_BE/public/dskh_template.xlsx
+++ b/BE/hix_lix_BE/public/dskh_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\LIX-HIX\hixlix_fe\BE\hix_lix_BE\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7528575-4099-4AFF-9143-2CACAA4D07E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5FEC3-40DE-4E60-9291-75C293202F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Danh sách KH" sheetId="1" r:id="rId1"/>
+    <sheet name="Danh sách PKS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ĐƠN VỊ: VIỄN THÔNG HẬU GIANG</t>
   </si>
   <si>
-    <t xml:space="preserve">DANH SÁCH BÁO CÁO </t>
-  </si>
-  <si>
     <t>Tỉnh</t>
   </si>
   <si>
@@ -96,12 +93,24 @@
   </si>
   <si>
     <t>Nhân viên thu cước</t>
+  </si>
+  <si>
+    <t>DANH SÁCH PHIẾU KHẢO SÁT</t>
+  </si>
+  <si>
+    <t>Thời gian lắp đặt</t>
+  </si>
+  <si>
+    <t>Thời gian ngưng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ [$₫-42A]_-;\-* #,##0\ [$₫-42A]_-;_-* &quot;-&quot;??\ [$₫-42A]_-;_-@_-"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,22 +188,29 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -537,137 +553,151 @@
     <col min="12" max="12" width="14.69921875" customWidth="1"/>
     <col min="13" max="13" width="14.3984375" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="14.19921875" customWidth="1"/>
+    <col min="15" max="15" width="14.19921875" style="11" customWidth="1"/>
     <col min="16" max="16" width="14.09765625" customWidth="1"/>
     <col min="17" max="17" width="14.59765625" customWidth="1"/>
     <col min="18" max="18" width="13.59765625" customWidth="1"/>
-    <col min="19" max="19" width="18.296875" customWidth="1"/>
+    <col min="19" max="19" width="14.296875" customWidth="1"/>
+    <col min="20" max="20" width="13.59765625" customWidth="1"/>
+    <col min="21" max="21" width="18.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+    </row>
+    <row r="3" spans="1:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="7" spans="1:21" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
+    <row r="8" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="O8" s="13"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q11" s="7"/>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:S3"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A2:U3"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated new code for bugs fix
</commit_message>
<xml_diff>
--- a/BE/hix_lix_BE/public/dskh_template.xlsx
+++ b/BE/hix_lix_BE/public/dskh_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\LIX-HIX\hixlix_fe\BE\hix_lix_BE\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463B4454-1F64-48BA-8896-8A46B45AE930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3C1378-4FB3-4CEF-A6F7-A216F054127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -546,14 +546,14 @@
     <col min="2" max="2" width="21.59765625" customWidth="1"/>
     <col min="3" max="3" width="22.796875" customWidth="1"/>
     <col min="4" max="4" width="20.19921875" customWidth="1"/>
-    <col min="5" max="5" width="26.59765625" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="35.296875" customWidth="1"/>
     <col min="7" max="7" width="19.19921875" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="21.09765625" customWidth="1"/>
+    <col min="10" max="10" width="26.296875" customWidth="1"/>
     <col min="11" max="11" width="19.69921875" customWidth="1"/>
-    <col min="12" max="12" width="14.69921875" customWidth="1"/>
+    <col min="12" max="12" width="22.19921875" customWidth="1"/>
     <col min="13" max="13" width="14.3984375" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
     <col min="15" max="15" width="14.19921875" style="11" customWidth="1"/>
@@ -563,7 +563,7 @@
     <col min="19" max="19" width="14.296875" customWidth="1"/>
     <col min="20" max="20" width="13.59765625" customWidth="1"/>
     <col min="21" max="21" width="18.296875" customWidth="1"/>
-    <col min="22" max="22" width="17.69921875" customWidth="1"/>
+    <col min="22" max="22" width="30.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>